<commit_message>
swapped UART rx&tx to match the UD3
</commit_message>
<xml_diff>
--- a/Project Outputs for UD3 Fibernet/UD3 Fibernet.xlsx
+++ b/Project Outputs for UD3 Fibernet/UD3 Fibernet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\OICE_16_974FA576_32C1D314_2E5C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68fbceef49caa884/Altium/Projects/UD3_Fibernet/Project Outputs for UD3 Fibernet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F02E9F1-9780-4855-AF24-3C48D68CA488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{5F02E9F1-9780-4855-AF24-3C48D68CA488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F68A1916-60C9-4B64-9C26-AF5317821A40}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{3D74BF8C-77F1-4C83-9DD6-540AC7B61EB4}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" xr2:uid="{3D74BF8C-77F1-4C83-9DD6-540AC7B61EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="UD3 Fibernet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="112">
   <si>
     <t>Line #</t>
   </si>
@@ -98,18 +98,12 @@
     <t>0,0172</t>
   </si>
   <si>
-    <t>0,39566</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
     <t>C6, C7, C9, C16, C17, C19, C35, C37</t>
   </si>
   <si>
-    <t>0,17203</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -209,18 +203,12 @@
     <t>0,1177</t>
   </si>
   <si>
-    <t>0,58851</t>
-  </si>
-  <si>
     <t>1uH</t>
   </si>
   <si>
     <t>L5, L6</t>
   </si>
   <si>
-    <t>0,2354</t>
-  </si>
-  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -234,9 +222,6 @@
   </si>
   <si>
     <t>0,01086</t>
-  </si>
-  <si>
-    <t>0,10865</t>
   </si>
   <si>
     <t>49.9</t>
@@ -455,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -463,6 +448,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -482,7 +468,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -778,9 +764,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CAF062-C8D6-4D85-8445-39BBB8C6B03B}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -798,7 +786,7 @@
     <col min="12" max="12" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,7 +824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -870,22 +858,22 @@
       <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="3">
+        <v>0.39566000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E3" s="3">
         <v>8</v>
@@ -908,22 +896,26 @@
       <c r="K3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="5">
+        <v>0.17202999999999999</v>
+      </c>
+      <c r="N3">
+        <f>SUM(L2:L27)</f>
+        <v>15.075669999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E4" s="3">
         <v>7</v>
@@ -946,60 +938,60 @@
       <c r="K4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="5">
+        <v>0.17202999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="K5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="L5" s="5">
+        <v>9.0539999999999995E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
@@ -1022,107 +1014,107 @@
       <c r="K6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="5">
+        <v>0.17202999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="K7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="5">
+        <v>9.0539999999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="I8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="K8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="5">
+        <v>9.0539999999999995E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>17</v>
@@ -1131,74 +1123,74 @@
         <v>18</v>
       </c>
       <c r="J9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.12676000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="K10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="4" t="s">
+      <c r="L10" s="5">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E11" s="3">
         <v>5</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>17</v>
@@ -1207,36 +1199,36 @@
         <v>18</v>
       </c>
       <c r="J11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0.58850999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E12" s="3">
         <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>17</v>
@@ -1245,27 +1237,27 @@
         <v>18</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.2354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E13" s="3">
         <v>5</v>
@@ -1274,7 +1266,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>17</v>
@@ -1283,27 +1275,27 @@
         <v>18</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0.10865</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
@@ -1312,7 +1304,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>17</v>
@@ -1321,27 +1313,27 @@
         <v>18</v>
       </c>
       <c r="J14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0.10865</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="E15" s="3">
         <v>2</v>
@@ -1350,7 +1342,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>17</v>
@@ -1359,27 +1351,27 @@
         <v>18</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0.10865</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E16" s="3">
         <v>2</v>
@@ -1388,7 +1380,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>17</v>
@@ -1397,13 +1389,13 @@
         <v>18</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0.10865</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1411,13 +1403,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E17" s="3">
         <v>7</v>
@@ -1426,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>17</v>
@@ -1435,13 +1427,13 @@
         <v>18</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0.10865</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1449,13 +1441,13 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -1464,7 +1456,7 @@
         <v>15</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>17</v>
@@ -1473,13 +1465,13 @@
         <v>18</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="L18" s="5">
+        <v>9.0539999999999995E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1487,13 +1479,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -1502,7 +1494,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>17</v>
@@ -1511,13 +1503,13 @@
         <v>18</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="L19" s="5">
+        <v>9.0539999999999995E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1525,13 +1517,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -1559,22 +1551,22 @@
         <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>17</v>
@@ -1583,32 +1575,34 @@
         <v>18</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="L21" s="3">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>17</v>
@@ -1617,32 +1611,34 @@
         <v>18</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="L22" s="3">
+        <v>5.13</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>17</v>
@@ -1651,13 +1647,13 @@
         <v>18</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
+      </c>
+      <c r="L23" s="5">
+        <v>3.44</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1665,13 +1661,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -1699,13 +1695,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -1733,13 +1729,13 @@
         <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1767,22 +1763,22 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>17</v>
@@ -1791,13 +1787,13 @@
         <v>18</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="L27" s="5">
+        <v>0.88729999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>